<commit_message>
calculated occupancy, train model must remove nan from appearing in station name
</commit_message>
<xml_diff>
--- a/track_model/block_information.xlsx
+++ b/track_model/block_information.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadin\Desktop\PlanesOverTrains\track_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60334520-5CBB-4AF3-A103-991C3285863E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86BC0C56-619B-4DF3-AFE4-4049B154442B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{2B483B09-FFFC-4D34-ABD1-C01B931B0F20}"/>
+    <workbookView xWindow="5430" yWindow="4245" windowWidth="21600" windowHeight="11235" xr2:uid="{2B483B09-FFFC-4D34-ABD1-C01B931B0F20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="69">
   <si>
     <t>line color</t>
   </si>
@@ -192,6 +192,57 @@
   </si>
   <si>
     <t>Station: Edgebrook (Left)</t>
+  </si>
+  <si>
+    <t>station side</t>
+  </si>
+  <si>
+    <t>Left/Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left </t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Station</t>
+  </si>
+  <si>
+    <t>Station: Whited</t>
+  </si>
+  <si>
+    <t>Station: South Bank</t>
+  </si>
+  <si>
+    <t>Station: Central</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Station: Inglewood</t>
+  </si>
+  <si>
+    <t>Station: Overbrook</t>
+  </si>
+  <si>
+    <t>Station: Glenbury</t>
+  </si>
+  <si>
+    <t>Station: Dormont</t>
+  </si>
+  <si>
+    <t>Station: Mt Lebanon</t>
+  </si>
+  <si>
+    <t>Station: Poplar</t>
+  </si>
+  <si>
+    <t>Station: Castle Shannon</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -552,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA592A9B-DE73-4643-A9BC-018E16FBEA2A}">
-  <dimension ref="A1:J242"/>
+  <dimension ref="A1:K242"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J101" sqref="J101"/>
+      <selection activeCell="K242" sqref="K1:K242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,9 +618,10 @@
     <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -600,8 +652,11 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -629,8 +684,14 @@
       <c r="I2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -658,8 +719,14 @@
       <c r="I3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -687,8 +754,14 @@
       <c r="I4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -716,8 +789,14 @@
       <c r="I5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -745,8 +824,14 @@
       <c r="I6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>68</v>
+      </c>
+      <c r="K6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -774,8 +859,14 @@
       <c r="I7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -803,8 +894,14 @@
       <c r="I8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>68</v>
+      </c>
+      <c r="K8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -832,8 +929,14 @@
       <c r="I9" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>68</v>
+      </c>
+      <c r="K9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -861,8 +964,14 @@
       <c r="I10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>68</v>
+      </c>
+      <c r="K10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -893,8 +1002,11 @@
       <c r="J11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -922,8 +1034,14 @@
       <c r="I12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -951,8 +1069,14 @@
       <c r="I13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -980,8 +1104,14 @@
       <c r="I14" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>68</v>
+      </c>
+      <c r="K14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1009,8 +1139,14 @@
       <c r="I15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>68</v>
+      </c>
+      <c r="K15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1041,8 +1177,11 @@
       <c r="J16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1070,8 +1209,14 @@
       <c r="I17" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>68</v>
+      </c>
+      <c r="K17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1099,8 +1244,14 @@
       <c r="I18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>68</v>
+      </c>
+      <c r="K18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1128,8 +1279,14 @@
       <c r="I19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>68</v>
+      </c>
+      <c r="K19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1157,8 +1314,14 @@
       <c r="I20" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>68</v>
+      </c>
+      <c r="K20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1186,8 +1349,14 @@
       <c r="I21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>68</v>
+      </c>
+      <c r="K21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -1215,8 +1384,14 @@
       <c r="I22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>68</v>
+      </c>
+      <c r="K22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -1247,8 +1422,11 @@
       <c r="J23" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -1276,8 +1454,14 @@
       <c r="I24" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>68</v>
+      </c>
+      <c r="K24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -1305,8 +1489,14 @@
       <c r="I25" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -1334,8 +1524,14 @@
       <c r="I26" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>68</v>
+      </c>
+      <c r="K26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -1363,8 +1559,14 @@
       <c r="I27" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>68</v>
+      </c>
+      <c r="K27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -1392,8 +1594,14 @@
       <c r="I28" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>68</v>
+      </c>
+      <c r="K28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -1421,8 +1629,14 @@
       <c r="I29" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>68</v>
+      </c>
+      <c r="K29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -1450,8 +1664,14 @@
       <c r="I30" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>68</v>
+      </c>
+      <c r="K30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1479,8 +1699,14 @@
       <c r="I31" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>68</v>
+      </c>
+      <c r="K31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -1511,8 +1737,11 @@
       <c r="J32" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -1540,8 +1769,14 @@
       <c r="I33" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J33" t="s">
+        <v>68</v>
+      </c>
+      <c r="K33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -1569,8 +1804,14 @@
       <c r="I34" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>68</v>
+      </c>
+      <c r="K34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -1598,8 +1839,14 @@
       <c r="I35" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J35" t="s">
+        <v>68</v>
+      </c>
+      <c r="K35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -1627,8 +1874,14 @@
       <c r="I36" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
+        <v>68</v>
+      </c>
+      <c r="K36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -1659,8 +1912,11 @@
       <c r="J37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -1688,8 +1944,14 @@
       <c r="I38" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J38" t="s">
+        <v>68</v>
+      </c>
+      <c r="K38" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -1717,8 +1979,14 @@
       <c r="I39" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J39" t="s">
+        <v>68</v>
+      </c>
+      <c r="K39" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -1746,8 +2014,14 @@
       <c r="I40" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J40" t="s">
+        <v>68</v>
+      </c>
+      <c r="K40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -1778,8 +2052,11 @@
       <c r="J41" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K41" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>16</v>
       </c>
@@ -1807,8 +2084,14 @@
       <c r="I42" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J42" t="s">
+        <v>68</v>
+      </c>
+      <c r="K42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -1836,8 +2119,14 @@
       <c r="I43" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J43" t="s">
+        <v>68</v>
+      </c>
+      <c r="K43" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>16</v>
       </c>
@@ -1865,8 +2154,14 @@
       <c r="I44" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J44" t="s">
+        <v>68</v>
+      </c>
+      <c r="K44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>16</v>
       </c>
@@ -1894,8 +2189,14 @@
       <c r="I45" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J45" t="s">
+        <v>68</v>
+      </c>
+      <c r="K45" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -1923,8 +2224,14 @@
       <c r="I46" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J46" t="s">
+        <v>68</v>
+      </c>
+      <c r="K46" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>16</v>
       </c>
@@ -1952,8 +2259,14 @@
       <c r="I47" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J47" t="s">
+        <v>68</v>
+      </c>
+      <c r="K47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -1981,8 +2294,14 @@
       <c r="I48" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J48" t="s">
+        <v>68</v>
+      </c>
+      <c r="K48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -2010,8 +2329,14 @@
       <c r="I49" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J49" t="s">
+        <v>68</v>
+      </c>
+      <c r="K49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>16</v>
       </c>
@@ -2039,8 +2364,14 @@
       <c r="I50" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J50" t="s">
+        <v>68</v>
+      </c>
+      <c r="K50" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>16</v>
       </c>
@@ -2071,8 +2402,11 @@
       <c r="J51" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K51" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -2100,8 +2434,14 @@
       <c r="I52" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J52" t="s">
+        <v>68</v>
+      </c>
+      <c r="K52" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>16</v>
       </c>
@@ -2129,8 +2469,14 @@
       <c r="I53" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J53" t="s">
+        <v>68</v>
+      </c>
+      <c r="K53" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>16</v>
       </c>
@@ -2158,8 +2504,14 @@
       <c r="I54" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J54" t="s">
+        <v>68</v>
+      </c>
+      <c r="K54" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>16</v>
       </c>
@@ -2187,8 +2539,14 @@
       <c r="I55" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J55" t="s">
+        <v>68</v>
+      </c>
+      <c r="K55" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>16</v>
       </c>
@@ -2216,8 +2574,14 @@
       <c r="I56" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J56" t="s">
+        <v>68</v>
+      </c>
+      <c r="K56" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>16</v>
       </c>
@@ -2245,8 +2609,14 @@
       <c r="I57" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J57" t="s">
+        <v>68</v>
+      </c>
+      <c r="K57" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>16</v>
       </c>
@@ -2274,8 +2644,14 @@
       <c r="I58" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J58" t="s">
+        <v>68</v>
+      </c>
+      <c r="K58" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>16</v>
       </c>
@@ -2303,8 +2679,14 @@
       <c r="I59" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J59" t="s">
+        <v>68</v>
+      </c>
+      <c r="K59" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>16</v>
       </c>
@@ -2332,8 +2714,14 @@
       <c r="I60" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J60" t="s">
+        <v>68</v>
+      </c>
+      <c r="K60" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -2364,8 +2752,11 @@
       <c r="J61" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K61" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>16</v>
       </c>
@@ -2393,8 +2784,14 @@
       <c r="I62" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J62" t="s">
+        <v>68</v>
+      </c>
+      <c r="K62" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>16</v>
       </c>
@@ -2425,8 +2822,11 @@
       <c r="J63" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K63" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>16</v>
       </c>
@@ -2457,8 +2857,11 @@
       <c r="J64" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K64" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>16</v>
       </c>
@@ -2486,8 +2889,14 @@
       <c r="I65" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J65" t="s">
+        <v>68</v>
+      </c>
+      <c r="K65" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>16</v>
       </c>
@@ -2515,8 +2924,14 @@
       <c r="I66" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J66" t="s">
+        <v>68</v>
+      </c>
+      <c r="K66" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>16</v>
       </c>
@@ -2544,8 +2959,14 @@
       <c r="I67" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J67" t="s">
+        <v>68</v>
+      </c>
+      <c r="K67" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>16</v>
       </c>
@@ -2573,8 +2994,14 @@
       <c r="I68" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J68" t="s">
+        <v>68</v>
+      </c>
+      <c r="K68" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>16</v>
       </c>
@@ -2602,8 +3029,14 @@
       <c r="I69" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J69" t="s">
+        <v>68</v>
+      </c>
+      <c r="K69" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>16</v>
       </c>
@@ -2631,8 +3064,14 @@
       <c r="I70" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J70" t="s">
+        <v>68</v>
+      </c>
+      <c r="K70" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>16</v>
       </c>
@@ -2660,8 +3099,14 @@
       <c r="I71" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J71" t="s">
+        <v>68</v>
+      </c>
+      <c r="K71" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>16</v>
       </c>
@@ -2689,8 +3134,14 @@
       <c r="I72" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J72" t="s">
+        <v>68</v>
+      </c>
+      <c r="K72" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>16</v>
       </c>
@@ -2718,8 +3169,14 @@
       <c r="I73" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J73" t="s">
+        <v>68</v>
+      </c>
+      <c r="K73" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>16</v>
       </c>
@@ -2747,8 +3204,14 @@
       <c r="I74" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J74" t="s">
+        <v>68</v>
+      </c>
+      <c r="K74" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>16</v>
       </c>
@@ -2776,8 +3239,14 @@
       <c r="I75" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J75" t="s">
+        <v>68</v>
+      </c>
+      <c r="K75" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>16</v>
       </c>
@@ -2808,8 +3277,11 @@
       <c r="J76" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K76" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>16</v>
       </c>
@@ -2837,8 +3309,14 @@
       <c r="I77" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J77" t="s">
+        <v>68</v>
+      </c>
+      <c r="K77" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>16</v>
       </c>
@@ -2866,8 +3344,14 @@
       <c r="I78" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J78" t="s">
+        <v>68</v>
+      </c>
+      <c r="K78" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>16</v>
       </c>
@@ -2895,8 +3379,14 @@
       <c r="I79" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J79" t="s">
+        <v>68</v>
+      </c>
+      <c r="K79" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>16</v>
       </c>
@@ -2924,8 +3414,14 @@
       <c r="I80" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J80" t="s">
+        <v>68</v>
+      </c>
+      <c r="K80" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>16</v>
       </c>
@@ -2953,8 +3449,14 @@
       <c r="I81" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J81" t="s">
+        <v>68</v>
+      </c>
+      <c r="K81" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>16</v>
       </c>
@@ -2982,8 +3484,14 @@
       <c r="I82" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J82" t="s">
+        <v>68</v>
+      </c>
+      <c r="K82" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>16</v>
       </c>
@@ -3011,8 +3519,14 @@
       <c r="I83" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J83" t="s">
+        <v>68</v>
+      </c>
+      <c r="K83" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>16</v>
       </c>
@@ -3040,8 +3554,14 @@
       <c r="I84" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J84" t="s">
+        <v>68</v>
+      </c>
+      <c r="K84" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>16</v>
       </c>
@@ -3069,8 +3589,14 @@
       <c r="I85" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J85" t="s">
+        <v>68</v>
+      </c>
+      <c r="K85" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>16</v>
       </c>
@@ -3098,8 +3624,14 @@
       <c r="I86" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J86" t="s">
+        <v>68</v>
+      </c>
+      <c r="K86" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>16</v>
       </c>
@@ -3127,8 +3659,14 @@
       <c r="I87" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J87" t="s">
+        <v>68</v>
+      </c>
+      <c r="K87" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>16</v>
       </c>
@@ -3156,8 +3694,14 @@
       <c r="I88" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J88" t="s">
+        <v>68</v>
+      </c>
+      <c r="K88" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>16</v>
       </c>
@@ -3185,8 +3729,14 @@
       <c r="I89" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J89" t="s">
+        <v>68</v>
+      </c>
+      <c r="K89" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>16</v>
       </c>
@@ -3214,8 +3764,14 @@
       <c r="I90" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J90" t="s">
+        <v>68</v>
+      </c>
+      <c r="K90" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>16</v>
       </c>
@@ -3243,8 +3799,14 @@
       <c r="I91" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J91" t="s">
+        <v>68</v>
+      </c>
+      <c r="K91" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>16</v>
       </c>
@@ -3272,8 +3834,14 @@
       <c r="I92" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J92" t="s">
+        <v>68</v>
+      </c>
+      <c r="K92" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>43</v>
       </c>
@@ -3301,8 +3869,14 @@
       <c r="I93" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J93" t="s">
+        <v>68</v>
+      </c>
+      <c r="K93" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>43</v>
       </c>
@@ -3333,8 +3907,11 @@
       <c r="J94" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K94" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>43</v>
       </c>
@@ -3362,8 +3939,14 @@
       <c r="I95" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J95" t="s">
+        <v>68</v>
+      </c>
+      <c r="K95" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>43</v>
       </c>
@@ -3391,8 +3974,14 @@
       <c r="I96" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J96" t="s">
+        <v>68</v>
+      </c>
+      <c r="K96" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>43</v>
       </c>
@@ -3420,8 +4009,14 @@
       <c r="I97" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J97" t="s">
+        <v>68</v>
+      </c>
+      <c r="K97" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>43</v>
       </c>
@@ -3449,8 +4044,14 @@
       <c r="I98" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J98" t="s">
+        <v>68</v>
+      </c>
+      <c r="K98" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>43</v>
       </c>
@@ -3478,8 +4079,14 @@
       <c r="I99" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J99" t="s">
+        <v>68</v>
+      </c>
+      <c r="K99" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>43</v>
       </c>
@@ -3507,8 +4114,14 @@
       <c r="I100" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J100" t="s">
+        <v>68</v>
+      </c>
+      <c r="K100" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>43</v>
       </c>
@@ -3539,8 +4152,11 @@
       <c r="J101" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K101" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>43</v>
       </c>
@@ -3568,8 +4184,14 @@
       <c r="I102" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J102" t="s">
+        <v>68</v>
+      </c>
+      <c r="K102" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>43</v>
       </c>
@@ -3597,8 +4219,14 @@
       <c r="I103" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J103" t="s">
+        <v>68</v>
+      </c>
+      <c r="K103" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>43</v>
       </c>
@@ -3626,8 +4254,14 @@
       <c r="I104" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J104" t="s">
+        <v>68</v>
+      </c>
+      <c r="K104" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>43</v>
       </c>
@@ -3655,8 +4289,14 @@
       <c r="I105" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J105" t="s">
+        <v>68</v>
+      </c>
+      <c r="K105" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>43</v>
       </c>
@@ -3684,8 +4324,14 @@
       <c r="I106" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J106" t="s">
+        <v>68</v>
+      </c>
+      <c r="K106" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>43</v>
       </c>
@@ -3713,8 +4359,14 @@
       <c r="I107" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J107" t="s">
+        <v>68</v>
+      </c>
+      <c r="K107" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>43</v>
       </c>
@@ -3742,8 +4394,14 @@
       <c r="I108" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J108" t="s">
+        <v>56</v>
+      </c>
+      <c r="K108" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>43</v>
       </c>
@@ -3771,8 +4429,14 @@
       <c r="I109" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J109" t="s">
+        <v>68</v>
+      </c>
+      <c r="K109" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>43</v>
       </c>
@@ -3800,8 +4464,14 @@
       <c r="I110" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J110" t="s">
+        <v>68</v>
+      </c>
+      <c r="K110" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>43</v>
       </c>
@@ -3829,8 +4499,14 @@
       <c r="I111" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J111" t="s">
+        <v>68</v>
+      </c>
+      <c r="K111" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>43</v>
       </c>
@@ -3858,8 +4534,14 @@
       <c r="I112" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J112" t="s">
+        <v>68</v>
+      </c>
+      <c r="K112" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>43</v>
       </c>
@@ -3887,8 +4569,14 @@
       <c r="I113" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J113" t="s">
+        <v>68</v>
+      </c>
+      <c r="K113" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>43</v>
       </c>
@@ -3916,8 +4604,14 @@
       <c r="I114" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J114" t="s">
+        <v>57</v>
+      </c>
+      <c r="K114" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>43</v>
       </c>
@@ -3945,8 +4639,14 @@
       <c r="I115" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J115" t="s">
+        <v>68</v>
+      </c>
+      <c r="K115" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>43</v>
       </c>
@@ -3974,8 +4674,14 @@
       <c r="I116" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J116" t="s">
+        <v>68</v>
+      </c>
+      <c r="K116" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>43</v>
       </c>
@@ -4003,8 +4709,14 @@
       <c r="I117" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J117" t="s">
+        <v>68</v>
+      </c>
+      <c r="K117" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>43</v>
       </c>
@@ -4032,8 +4744,14 @@
       <c r="I118" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J118" t="s">
+        <v>68</v>
+      </c>
+      <c r="K118" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>43</v>
       </c>
@@ -4061,8 +4779,14 @@
       <c r="I119" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J119" t="s">
+        <v>68</v>
+      </c>
+      <c r="K119" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>43</v>
       </c>
@@ -4090,8 +4814,14 @@
       <c r="I120" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J120" t="s">
+        <v>68</v>
+      </c>
+      <c r="K120" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>43</v>
       </c>
@@ -4119,8 +4849,14 @@
       <c r="I121" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J121" t="s">
+        <v>68</v>
+      </c>
+      <c r="K121" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>43</v>
       </c>
@@ -4148,8 +4884,14 @@
       <c r="I122" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J122" t="s">
+        <v>68</v>
+      </c>
+      <c r="K122" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>43</v>
       </c>
@@ -4177,8 +4919,14 @@
       <c r="I123" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J123" t="s">
+        <v>58</v>
+      </c>
+      <c r="K123" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>43</v>
       </c>
@@ -4206,8 +4954,14 @@
       <c r="I124" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J124" t="s">
+        <v>68</v>
+      </c>
+      <c r="K124" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>43</v>
       </c>
@@ -4235,8 +4989,14 @@
       <c r="I125" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J125" t="s">
+        <v>68</v>
+      </c>
+      <c r="K125" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>43</v>
       </c>
@@ -4264,8 +5024,14 @@
       <c r="I126" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J126" t="s">
+        <v>68</v>
+      </c>
+      <c r="K126" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>43</v>
       </c>
@@ -4293,8 +5059,14 @@
       <c r="I127" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J127" t="s">
+        <v>68</v>
+      </c>
+      <c r="K127" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>43</v>
       </c>
@@ -4322,8 +5094,14 @@
       <c r="I128" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J128" t="s">
+        <v>68</v>
+      </c>
+      <c r="K128" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>43</v>
       </c>
@@ -4351,8 +5129,14 @@
       <c r="I129" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J129" t="s">
+        <v>68</v>
+      </c>
+      <c r="K129" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>43</v>
       </c>
@@ -4380,8 +5164,14 @@
       <c r="I130" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J130" t="s">
+        <v>59</v>
+      </c>
+      <c r="K130" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>43</v>
       </c>
@@ -4409,8 +5199,14 @@
       <c r="I131" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J131" t="s">
+        <v>68</v>
+      </c>
+      <c r="K131" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>43</v>
       </c>
@@ -4438,8 +5234,14 @@
       <c r="I132" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J132" t="s">
+        <v>68</v>
+      </c>
+      <c r="K132" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>43</v>
       </c>
@@ -4467,8 +5269,14 @@
       <c r="I133" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J133" t="s">
+        <v>68</v>
+      </c>
+      <c r="K133" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>43</v>
       </c>
@@ -4496,8 +5304,14 @@
       <c r="I134" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J134" t="s">
+        <v>68</v>
+      </c>
+      <c r="K134" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>43</v>
       </c>
@@ -4525,8 +5339,14 @@
       <c r="I135" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J135" t="s">
+        <v>68</v>
+      </c>
+      <c r="K135" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>43</v>
       </c>
@@ -4554,8 +5374,14 @@
       <c r="I136" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J136" t="s">
+        <v>68</v>
+      </c>
+      <c r="K136" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>43</v>
       </c>
@@ -4583,8 +5409,14 @@
       <c r="I137" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J137" t="s">
+        <v>68</v>
+      </c>
+      <c r="K137" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>43</v>
       </c>
@@ -4612,8 +5444,14 @@
       <c r="I138" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J138" t="s">
+        <v>68</v>
+      </c>
+      <c r="K138" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>43</v>
       </c>
@@ -4641,8 +5479,14 @@
       <c r="I139" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J139" t="s">
+        <v>61</v>
+      </c>
+      <c r="K139" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>43</v>
       </c>
@@ -4670,8 +5514,14 @@
       <c r="I140" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J140" t="s">
+        <v>68</v>
+      </c>
+      <c r="K140" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>43</v>
       </c>
@@ -4699,8 +5549,14 @@
       <c r="I141" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J141" t="s">
+        <v>68</v>
+      </c>
+      <c r="K141" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>43</v>
       </c>
@@ -4728,8 +5584,14 @@
       <c r="I142" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J142" t="s">
+        <v>68</v>
+      </c>
+      <c r="K142" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>43</v>
       </c>
@@ -4757,8 +5619,14 @@
       <c r="I143" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J143" t="s">
+        <v>68</v>
+      </c>
+      <c r="K143" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>43</v>
       </c>
@@ -4786,8 +5654,14 @@
       <c r="I144" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J144" t="s">
+        <v>68</v>
+      </c>
+      <c r="K144" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>43</v>
       </c>
@@ -4815,8 +5689,14 @@
       <c r="I145" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J145" t="s">
+        <v>68</v>
+      </c>
+      <c r="K145" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>43</v>
       </c>
@@ -4844,8 +5724,14 @@
       <c r="I146" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J146" t="s">
+        <v>68</v>
+      </c>
+      <c r="K146" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>43</v>
       </c>
@@ -4873,8 +5759,14 @@
       <c r="I147" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J147" t="s">
+        <v>68</v>
+      </c>
+      <c r="K147" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>43</v>
       </c>
@@ -4902,8 +5794,14 @@
       <c r="I148" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J148" t="s">
+        <v>62</v>
+      </c>
+      <c r="K148" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>43</v>
       </c>
@@ -4931,8 +5829,14 @@
       <c r="I149" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J149" t="s">
+        <v>68</v>
+      </c>
+      <c r="K149" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>43</v>
       </c>
@@ -4960,8 +5864,14 @@
       <c r="I150" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J150" t="s">
+        <v>68</v>
+      </c>
+      <c r="K150" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>43</v>
       </c>
@@ -4989,8 +5899,14 @@
       <c r="I151" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J151" t="s">
+        <v>68</v>
+      </c>
+      <c r="K151" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>43</v>
       </c>
@@ -5018,8 +5934,14 @@
       <c r="I152" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J152" t="s">
+        <v>68</v>
+      </c>
+      <c r="K152" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>43</v>
       </c>
@@ -5047,8 +5969,14 @@
       <c r="I153" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J153" t="s">
+        <v>68</v>
+      </c>
+      <c r="K153" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>43</v>
       </c>
@@ -5076,8 +6004,14 @@
       <c r="I154" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J154" t="s">
+        <v>68</v>
+      </c>
+      <c r="K154" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>43</v>
       </c>
@@ -5105,8 +6039,14 @@
       <c r="I155" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J155" t="s">
+        <v>68</v>
+      </c>
+      <c r="K155" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>43</v>
       </c>
@@ -5134,8 +6074,14 @@
       <c r="I156" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J156" t="s">
+        <v>68</v>
+      </c>
+      <c r="K156" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>43</v>
       </c>
@@ -5163,8 +6109,14 @@
       <c r="I157" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J157" t="s">
+        <v>63</v>
+      </c>
+      <c r="K157" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>43</v>
       </c>
@@ -5192,8 +6144,14 @@
       <c r="I158" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J158" t="s">
+        <v>68</v>
+      </c>
+      <c r="K158" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>43</v>
       </c>
@@ -5221,8 +6179,14 @@
       <c r="I159" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J159" t="s">
+        <v>68</v>
+      </c>
+      <c r="K159" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>43</v>
       </c>
@@ -5250,8 +6214,14 @@
       <c r="I160" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J160" t="s">
+        <v>68</v>
+      </c>
+      <c r="K160" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>43</v>
       </c>
@@ -5279,8 +6249,14 @@
       <c r="I161" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J161" t="s">
+        <v>68</v>
+      </c>
+      <c r="K161" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>43</v>
       </c>
@@ -5308,8 +6284,14 @@
       <c r="I162" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J162" t="s">
+        <v>68</v>
+      </c>
+      <c r="K162" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>43</v>
       </c>
@@ -5337,8 +6319,14 @@
       <c r="I163" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J163" t="s">
+        <v>68</v>
+      </c>
+      <c r="K163" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>43</v>
       </c>
@@ -5366,8 +6354,14 @@
       <c r="I164" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J164" t="s">
+        <v>68</v>
+      </c>
+      <c r="K164" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>43</v>
       </c>
@@ -5395,8 +6389,14 @@
       <c r="I165" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J165" t="s">
+        <v>64</v>
+      </c>
+      <c r="K165" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>43</v>
       </c>
@@ -5424,8 +6424,14 @@
       <c r="I166" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J166" t="s">
+        <v>68</v>
+      </c>
+      <c r="K166" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>43</v>
       </c>
@@ -5453,8 +6459,14 @@
       <c r="I167" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J167" t="s">
+        <v>68</v>
+      </c>
+      <c r="K167" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>43</v>
       </c>
@@ -5482,8 +6494,14 @@
       <c r="I168" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J168" t="s">
+        <v>68</v>
+      </c>
+      <c r="K168" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>43</v>
       </c>
@@ -5511,8 +6529,14 @@
       <c r="I169" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J169" t="s">
+        <v>65</v>
+      </c>
+      <c r="K169" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>43</v>
       </c>
@@ -5540,8 +6564,14 @@
       <c r="I170" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J170" t="s">
+        <v>68</v>
+      </c>
+      <c r="K170" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>43</v>
       </c>
@@ -5569,8 +6599,14 @@
       <c r="I171" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J171" t="s">
+        <v>68</v>
+      </c>
+      <c r="K171" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>43</v>
       </c>
@@ -5598,8 +6634,14 @@
       <c r="I172" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J172" t="s">
+        <v>68</v>
+      </c>
+      <c r="K172" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>43</v>
       </c>
@@ -5627,8 +6669,14 @@
       <c r="I173" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J173" t="s">
+        <v>68</v>
+      </c>
+      <c r="K173" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>43</v>
       </c>
@@ -5656,8 +6704,14 @@
       <c r="I174" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J174" t="s">
+        <v>68</v>
+      </c>
+      <c r="K174" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>43</v>
       </c>
@@ -5685,8 +6739,14 @@
       <c r="I175" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J175" t="s">
+        <v>68</v>
+      </c>
+      <c r="K175" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>43</v>
       </c>
@@ -5714,8 +6774,14 @@
       <c r="I176" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J176" t="s">
+        <v>68</v>
+      </c>
+      <c r="K176" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>43</v>
       </c>
@@ -5743,8 +6809,14 @@
       <c r="I177" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J177" t="s">
+        <v>68</v>
+      </c>
+      <c r="K177" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>43</v>
       </c>
@@ -5772,8 +6844,14 @@
       <c r="I178" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J178" t="s">
+        <v>68</v>
+      </c>
+      <c r="K178" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>43</v>
       </c>
@@ -5801,8 +6879,14 @@
       <c r="I179" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J179" t="s">
+        <v>68</v>
+      </c>
+      <c r="K179" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>43</v>
       </c>
@@ -5830,8 +6914,14 @@
       <c r="I180" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J180" t="s">
+        <v>66</v>
+      </c>
+      <c r="K180" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>43</v>
       </c>
@@ -5859,8 +6949,14 @@
       <c r="I181" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J181" t="s">
+        <v>68</v>
+      </c>
+      <c r="K181" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>43</v>
       </c>
@@ -5888,8 +6984,14 @@
       <c r="I182" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J182" t="s">
+        <v>68</v>
+      </c>
+      <c r="K182" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>43</v>
       </c>
@@ -5917,8 +7019,14 @@
       <c r="I183" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J183" t="s">
+        <v>68</v>
+      </c>
+      <c r="K183" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>43</v>
       </c>
@@ -5946,8 +7054,14 @@
       <c r="I184" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J184" t="s">
+        <v>68</v>
+      </c>
+      <c r="K184" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>43</v>
       </c>
@@ -5975,8 +7089,14 @@
       <c r="I185" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J185" t="s">
+        <v>68</v>
+      </c>
+      <c r="K185" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>43</v>
       </c>
@@ -6004,8 +7124,14 @@
       <c r="I186" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J186" t="s">
+        <v>68</v>
+      </c>
+      <c r="K186" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>43</v>
       </c>
@@ -6033,8 +7159,14 @@
       <c r="I187" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J187" t="s">
+        <v>68</v>
+      </c>
+      <c r="K187" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>43</v>
       </c>
@@ -6062,8 +7194,14 @@
       <c r="I188" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J188" t="s">
+        <v>67</v>
+      </c>
+      <c r="K188" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>43</v>
       </c>
@@ -6091,8 +7229,14 @@
       <c r="I189" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J189" t="s">
+        <v>68</v>
+      </c>
+      <c r="K189" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>43</v>
       </c>
@@ -6120,8 +7264,14 @@
       <c r="I190" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J190" t="s">
+        <v>68</v>
+      </c>
+      <c r="K190" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>43</v>
       </c>
@@ -6149,8 +7299,14 @@
       <c r="I191" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J191" t="s">
+        <v>68</v>
+      </c>
+      <c r="K191" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>43</v>
       </c>
@@ -6178,8 +7334,14 @@
       <c r="I192" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J192" t="s">
+        <v>68</v>
+      </c>
+      <c r="K192" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>43</v>
       </c>
@@ -6207,8 +7369,14 @@
       <c r="I193" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J193" t="s">
+        <v>68</v>
+      </c>
+      <c r="K193" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>43</v>
       </c>
@@ -6236,8 +7404,14 @@
       <c r="I194" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J194" t="s">
+        <v>68</v>
+      </c>
+      <c r="K194" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>43</v>
       </c>
@@ -6265,8 +7439,14 @@
       <c r="I195" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J195" t="s">
+        <v>68</v>
+      </c>
+      <c r="K195" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>43</v>
       </c>
@@ -6294,8 +7474,14 @@
       <c r="I196" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J196" t="s">
+        <v>68</v>
+      </c>
+      <c r="K196" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>43</v>
       </c>
@@ -6323,8 +7509,14 @@
       <c r="I197" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J197" t="s">
+        <v>64</v>
+      </c>
+      <c r="K197" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>43</v>
       </c>
@@ -6352,8 +7544,14 @@
       <c r="I198" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J198" t="s">
+        <v>68</v>
+      </c>
+      <c r="K198" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>43</v>
       </c>
@@ -6381,8 +7579,14 @@
       <c r="I199" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J199" t="s">
+        <v>68</v>
+      </c>
+      <c r="K199" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>43</v>
       </c>
@@ -6410,8 +7614,14 @@
       <c r="I200" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J200" t="s">
+        <v>68</v>
+      </c>
+      <c r="K200" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>43</v>
       </c>
@@ -6439,8 +7649,14 @@
       <c r="I201" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J201" t="s">
+        <v>68</v>
+      </c>
+      <c r="K201" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>43</v>
       </c>
@@ -6468,8 +7684,14 @@
       <c r="I202" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J202" t="s">
+        <v>68</v>
+      </c>
+      <c r="K202" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>43</v>
       </c>
@@ -6497,8 +7719,14 @@
       <c r="I203" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J203" t="s">
+        <v>68</v>
+      </c>
+      <c r="K203" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>43</v>
       </c>
@@ -6526,8 +7754,14 @@
       <c r="I204" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J204" t="s">
+        <v>68</v>
+      </c>
+      <c r="K204" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>43</v>
       </c>
@@ -6555,8 +7789,14 @@
       <c r="I205" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J205" t="s">
+        <v>68</v>
+      </c>
+      <c r="K205" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>43</v>
       </c>
@@ -6584,8 +7824,14 @@
       <c r="I206" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J206" t="s">
+        <v>68</v>
+      </c>
+      <c r="K206" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>43</v>
       </c>
@@ -6613,8 +7859,14 @@
       <c r="I207" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J207" t="s">
+        <v>68</v>
+      </c>
+      <c r="K207" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>43</v>
       </c>
@@ -6642,8 +7894,14 @@
       <c r="I208" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J208" t="s">
+        <v>68</v>
+      </c>
+      <c r="K208" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>43</v>
       </c>
@@ -6671,8 +7929,14 @@
       <c r="I209" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J209" t="s">
+        <v>68</v>
+      </c>
+      <c r="K209" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>43</v>
       </c>
@@ -6700,8 +7964,14 @@
       <c r="I210" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J210" t="s">
+        <v>68</v>
+      </c>
+      <c r="K210" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>43</v>
       </c>
@@ -6729,8 +7999,14 @@
       <c r="I211" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J211" t="s">
+        <v>68</v>
+      </c>
+      <c r="K211" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>43</v>
       </c>
@@ -6758,8 +8034,14 @@
       <c r="I212" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J212" t="s">
+        <v>68</v>
+      </c>
+      <c r="K212" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>43</v>
       </c>
@@ -6787,8 +8069,14 @@
       <c r="I213" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J213" t="s">
+        <v>68</v>
+      </c>
+      <c r="K213" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>43</v>
       </c>
@@ -6816,8 +8104,14 @@
       <c r="I214" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J214" t="s">
+        <v>68</v>
+      </c>
+      <c r="K214" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>43</v>
       </c>
@@ -6845,8 +8139,14 @@
       <c r="I215" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J215" t="s">
+        <v>68</v>
+      </c>
+      <c r="K215" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>43</v>
       </c>
@@ -6874,8 +8174,14 @@
       <c r="I216" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J216" t="s">
+        <v>68</v>
+      </c>
+      <c r="K216" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>43</v>
       </c>
@@ -6903,8 +8209,14 @@
       <c r="I217" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J217" t="s">
+        <v>68</v>
+      </c>
+      <c r="K217" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>43</v>
       </c>
@@ -6932,8 +8244,14 @@
       <c r="I218" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J218" t="s">
+        <v>68</v>
+      </c>
+      <c r="K218" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>43</v>
       </c>
@@ -6961,8 +8279,14 @@
       <c r="I219" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J219" t="s">
+        <v>68</v>
+      </c>
+      <c r="K219" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>43</v>
       </c>
@@ -6990,8 +8314,14 @@
       <c r="I220" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J220" t="s">
+        <v>68</v>
+      </c>
+      <c r="K220" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>43</v>
       </c>
@@ -7019,8 +8349,14 @@
       <c r="I221" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J221" t="s">
+        <v>68</v>
+      </c>
+      <c r="K221" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>43</v>
       </c>
@@ -7048,8 +8384,14 @@
       <c r="I222" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J222" t="s">
+        <v>68</v>
+      </c>
+      <c r="K222" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>43</v>
       </c>
@@ -7077,8 +8419,14 @@
       <c r="I223" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J223" t="s">
+        <v>68</v>
+      </c>
+      <c r="K223" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>43</v>
       </c>
@@ -7106,8 +8454,14 @@
       <c r="I224" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J224" t="s">
+        <v>68</v>
+      </c>
+      <c r="K224" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>43</v>
       </c>
@@ -7135,8 +8489,14 @@
       <c r="I225" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J225" t="s">
+        <v>68</v>
+      </c>
+      <c r="K225" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>43</v>
       </c>
@@ -7164,8 +8524,14 @@
       <c r="I226" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J226" t="s">
+        <v>68</v>
+      </c>
+      <c r="K226" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>43</v>
       </c>
@@ -7193,8 +8559,14 @@
       <c r="I227" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J227" t="s">
+        <v>68</v>
+      </c>
+      <c r="K227" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>43</v>
       </c>
@@ -7222,8 +8594,14 @@
       <c r="I228" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J228" t="s">
+        <v>68</v>
+      </c>
+      <c r="K228" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>43</v>
       </c>
@@ -7251,8 +8629,14 @@
       <c r="I229" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J229" t="s">
+        <v>68</v>
+      </c>
+      <c r="K229" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>43</v>
       </c>
@@ -7280,8 +8664,14 @@
       <c r="I230" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J230" t="s">
+        <v>68</v>
+      </c>
+      <c r="K230" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>43</v>
       </c>
@@ -7309,8 +8699,14 @@
       <c r="I231" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J231" t="s">
+        <v>68</v>
+      </c>
+      <c r="K231" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>43</v>
       </c>
@@ -7338,8 +8734,14 @@
       <c r="I232" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J232" t="s">
+        <v>68</v>
+      </c>
+      <c r="K232" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>43</v>
       </c>
@@ -7367,8 +8769,14 @@
       <c r="I233" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J233" t="s">
+        <v>68</v>
+      </c>
+      <c r="K233" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>43</v>
       </c>
@@ -7396,8 +8804,14 @@
       <c r="I234" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J234" t="s">
+        <v>68</v>
+      </c>
+      <c r="K234" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>43</v>
       </c>
@@ -7425,8 +8839,14 @@
       <c r="I235" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J235" t="s">
+        <v>68</v>
+      </c>
+      <c r="K235" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>43</v>
       </c>
@@ -7454,8 +8874,14 @@
       <c r="I236" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J236" t="s">
+        <v>68</v>
+      </c>
+      <c r="K236" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>43</v>
       </c>
@@ -7483,8 +8909,14 @@
       <c r="I237" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J237" t="s">
+        <v>68</v>
+      </c>
+      <c r="K237" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>43</v>
       </c>
@@ -7512,8 +8944,14 @@
       <c r="I238" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J238" t="s">
+        <v>68</v>
+      </c>
+      <c r="K238" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>43</v>
       </c>
@@ -7541,8 +8979,14 @@
       <c r="I239" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J239" t="s">
+        <v>68</v>
+      </c>
+      <c r="K239" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>43</v>
       </c>
@@ -7570,8 +9014,14 @@
       <c r="I240" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J240" t="s">
+        <v>68</v>
+      </c>
+      <c r="K240" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>43</v>
       </c>
@@ -7599,8 +9049,14 @@
       <c r="I241" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J241" t="s">
+        <v>68</v>
+      </c>
+      <c r="K241" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>43</v>
       </c>
@@ -7627,6 +9083,12 @@
       </c>
       <c r="I242" t="b">
         <v>0</v>
+      </c>
+      <c r="J242" t="s">
+        <v>68</v>
+      </c>
+      <c r="K242" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dont know if its working, serial stuff is in right now, need to push to get it on my laptop
</commit_message>
<xml_diff>
--- a/track_model/block_information.xlsx
+++ b/track_model/block_information.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadin\Desktop\PlanesOverTrains\track_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanr\PycharmProjects\PlanesOverTrains\track_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86BC0C56-619B-4DF3-AFE4-4049B154442B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BEDEC2-B3D3-4518-A4F7-4C5DE021DB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5430" yWindow="4245" windowWidth="21600" windowHeight="11235" xr2:uid="{2B483B09-FFFC-4D34-ABD1-C01B931B0F20}"/>
+    <workbookView xWindow="28680" yWindow="525" windowWidth="29040" windowHeight="15720" xr2:uid="{2B483B09-FFFC-4D34-ABD1-C01B931B0F20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -605,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA592A9B-DE73-4643-A9BC-018E16FBEA2A}">
   <dimension ref="A1:K242"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K242" sqref="K1:K242"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H177" sqref="H177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4249,7 +4249,7 @@
         <v>-3</v>
       </c>
       <c r="H104" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I104" t="b">
         <v>0</v>
@@ -4284,7 +4284,7 @@
         <v>0</v>
       </c>
       <c r="H105" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I105" t="b">
         <v>0</v>
@@ -4809,7 +4809,7 @@
         <v>0</v>
       </c>
       <c r="H120" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I120" t="b">
         <v>0</v>
@@ -4844,7 +4844,7 @@
         <v>0</v>
       </c>
       <c r="H121" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I121" t="b">
         <v>0</v>
@@ -5824,7 +5824,7 @@
         <v>0</v>
       </c>
       <c r="H149" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I149" t="b">
         <v>1</v>
@@ -5859,7 +5859,7 @@
         <v>0</v>
       </c>
       <c r="H150" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I150" t="b">
         <v>0</v>
@@ -6489,7 +6489,7 @@
         <v>0</v>
       </c>
       <c r="H168" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I168" t="b">
         <v>0</v>
@@ -6524,7 +6524,7 @@
         <v>0</v>
       </c>
       <c r="H169" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I169" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
added occupancy function in Track_Model_UI, tweaked UI format
</commit_message>
<xml_diff>
--- a/track_model/block_information.xlsx
+++ b/track_model/block_information.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanr\PycharmProjects\PlanesOverTrains\track_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadin\Desktop\PlanesOverTrains\track_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BEDEC2-B3D3-4518-A4F7-4C5DE021DB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2229E9D3-9F26-4AFE-A71A-C64721B9F5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="525" windowWidth="29040" windowHeight="15720" xr2:uid="{2B483B09-FFFC-4D34-ABD1-C01B931B0F20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B483B09-FFFC-4D34-ABD1-C01B931B0F20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="68">
   <si>
     <t>line color</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Station: First Ave</t>
   </si>
   <si>
-    <t>Railway Crossing</t>
-  </si>
-  <si>
     <t>Station: Station Square</t>
   </si>
   <si>
@@ -186,12 +183,6 @@
   </si>
   <si>
     <t>Z</t>
-  </si>
-  <si>
-    <t>Station: Pioneer (Left)</t>
-  </si>
-  <si>
-    <t>Station: Edgebrook (Left)</t>
   </si>
   <si>
     <t>station side</t>
@@ -243,6 +234,12 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>Station: Pioneer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Station: Edgebrook </t>
   </si>
 </sst>
 </file>
@@ -605,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA592A9B-DE73-4643-A9BC-018E16FBEA2A}">
   <dimension ref="A1:K242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H177" sqref="H177"/>
+    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
+      <selection activeCell="J101" sqref="J101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,7 +650,7 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -685,10 +682,10 @@
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -720,10 +717,10 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -755,10 +752,10 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -790,10 +787,10 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -825,10 +822,10 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -860,10 +857,10 @@
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -895,10 +892,10 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -930,10 +927,10 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -965,10 +962,10 @@
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1003,7 +1000,7 @@
         <v>14</v>
       </c>
       <c r="K11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1035,10 +1032,10 @@
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1070,10 +1067,10 @@
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1105,10 +1102,10 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1140,10 +1137,10 @@
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1178,7 +1175,7 @@
         <v>15</v>
       </c>
       <c r="K16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1210,10 +1207,10 @@
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1245,10 +1242,10 @@
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1280,10 +1277,10 @@
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K19" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1315,10 +1312,10 @@
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K20" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1350,10 +1347,10 @@
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K21" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1385,10 +1382,10 @@
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1423,7 +1420,7 @@
         <v>34</v>
       </c>
       <c r="K23" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1455,10 +1452,10 @@
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1490,10 +1487,10 @@
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K25" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1525,10 +1522,10 @@
         <v>0</v>
       </c>
       <c r="J26" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K26" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1560,10 +1557,10 @@
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K27" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1595,10 +1592,10 @@
         <v>0</v>
       </c>
       <c r="J28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1630,10 +1627,10 @@
         <v>0</v>
       </c>
       <c r="J29" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K29" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1665,10 +1662,10 @@
         <v>0</v>
       </c>
       <c r="J30" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K30" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1700,10 +1697,10 @@
         <v>0</v>
       </c>
       <c r="J31" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K31" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1738,7 +1735,7 @@
         <v>35</v>
       </c>
       <c r="K32" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -1770,10 +1767,10 @@
         <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K33" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -1805,10 +1802,10 @@
         <v>0</v>
       </c>
       <c r="J34" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K34" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -1840,10 +1837,10 @@
         <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K35" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -1875,10 +1872,10 @@
         <v>0</v>
       </c>
       <c r="J36" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K36" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -1913,7 +1910,7 @@
         <v>36</v>
       </c>
       <c r="K37" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -1945,10 +1942,10 @@
         <v>0</v>
       </c>
       <c r="J38" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K38" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -1980,10 +1977,10 @@
         <v>0</v>
       </c>
       <c r="J39" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K39" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2015,10 +2012,10 @@
         <v>1</v>
       </c>
       <c r="J40" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K40" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -2053,7 +2050,7 @@
         <v>37</v>
       </c>
       <c r="K41" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -2085,10 +2082,10 @@
         <v>1</v>
       </c>
       <c r="J42" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K42" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -2120,10 +2117,10 @@
         <v>1</v>
       </c>
       <c r="J43" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K43" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -2155,10 +2152,10 @@
         <v>1</v>
       </c>
       <c r="J44" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K44" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -2190,10 +2187,10 @@
         <v>1</v>
       </c>
       <c r="J45" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K45" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -2225,10 +2222,10 @@
         <v>1</v>
       </c>
       <c r="J46" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K46" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -2260,10 +2257,10 @@
         <v>1</v>
       </c>
       <c r="J47" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K47" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -2295,10 +2292,10 @@
         <v>1</v>
       </c>
       <c r="J48" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K48" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -2330,10 +2327,10 @@
         <v>1</v>
       </c>
       <c r="J49" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K49" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -2365,10 +2362,10 @@
         <v>1</v>
       </c>
       <c r="J50" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K50" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -2403,7 +2400,7 @@
         <v>38</v>
       </c>
       <c r="K51" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -2435,10 +2432,10 @@
         <v>1</v>
       </c>
       <c r="J52" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K52" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -2470,10 +2467,10 @@
         <v>1</v>
       </c>
       <c r="J53" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K53" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -2505,10 +2502,10 @@
         <v>1</v>
       </c>
       <c r="J54" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K54" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -2540,10 +2537,10 @@
         <v>1</v>
       </c>
       <c r="J55" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K55" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -2575,10 +2572,10 @@
         <v>1</v>
       </c>
       <c r="J56" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K56" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -2610,10 +2607,10 @@
         <v>1</v>
       </c>
       <c r="J57" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K57" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -2645,10 +2642,10 @@
         <v>1</v>
       </c>
       <c r="J58" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K58" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -2680,10 +2677,10 @@
         <v>1</v>
       </c>
       <c r="J59" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K59" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -2715,10 +2712,10 @@
         <v>1</v>
       </c>
       <c r="J60" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K60" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -2753,7 +2750,7 @@
         <v>39</v>
       </c>
       <c r="K61" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -2785,10 +2782,10 @@
         <v>1</v>
       </c>
       <c r="J62" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K62" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -2820,10 +2817,10 @@
         <v>0</v>
       </c>
       <c r="J63" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="K63" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -2855,10 +2852,10 @@
         <v>0</v>
       </c>
       <c r="J64" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K64" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
@@ -2890,10 +2887,10 @@
         <v>0</v>
       </c>
       <c r="J65" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K65" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
@@ -2925,10 +2922,10 @@
         <v>0</v>
       </c>
       <c r="J66" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K66" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
@@ -2960,10 +2957,10 @@
         <v>0</v>
       </c>
       <c r="J67" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K67" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -2995,10 +2992,10 @@
         <v>0</v>
       </c>
       <c r="J68" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K68" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
@@ -3030,10 +3027,10 @@
         <v>0</v>
       </c>
       <c r="J69" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K69" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -3065,10 +3062,10 @@
         <v>0</v>
       </c>
       <c r="J70" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K70" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
@@ -3100,10 +3097,10 @@
         <v>0</v>
       </c>
       <c r="J71" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K71" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
@@ -3135,10 +3132,10 @@
         <v>0</v>
       </c>
       <c r="J72" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K72" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
@@ -3170,10 +3167,10 @@
         <v>0</v>
       </c>
       <c r="J73" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K73" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
@@ -3205,10 +3202,10 @@
         <v>0</v>
       </c>
       <c r="J74" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K74" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -3240,10 +3237,10 @@
         <v>0</v>
       </c>
       <c r="J75" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K75" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
@@ -3275,10 +3272,10 @@
         <v>0</v>
       </c>
       <c r="J76" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K76" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
@@ -3310,10 +3307,10 @@
         <v>0</v>
       </c>
       <c r="J77" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K77" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
@@ -3345,10 +3342,10 @@
         <v>0</v>
       </c>
       <c r="J78" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K78" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
@@ -3380,10 +3377,10 @@
         <v>0</v>
       </c>
       <c r="J79" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K79" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
@@ -3415,10 +3412,10 @@
         <v>0</v>
       </c>
       <c r="J80" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K80" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
@@ -3450,10 +3447,10 @@
         <v>0</v>
       </c>
       <c r="J81" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K81" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -3485,10 +3482,10 @@
         <v>0</v>
       </c>
       <c r="J82" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K82" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
@@ -3520,10 +3517,10 @@
         <v>1</v>
       </c>
       <c r="J83" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K83" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
@@ -3555,10 +3552,10 @@
         <v>1</v>
       </c>
       <c r="J84" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K84" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
@@ -3590,10 +3587,10 @@
         <v>1</v>
       </c>
       <c r="J85" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K85" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
@@ -3625,10 +3622,10 @@
         <v>1</v>
       </c>
       <c r="J86" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K86" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
@@ -3660,10 +3657,10 @@
         <v>1</v>
       </c>
       <c r="J87" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K87" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
@@ -3695,10 +3692,10 @@
         <v>1</v>
       </c>
       <c r="J88" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K88" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
@@ -3730,10 +3727,10 @@
         <v>1</v>
       </c>
       <c r="J89" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K89" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
@@ -3765,10 +3762,10 @@
         <v>1</v>
       </c>
       <c r="J90" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K90" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
@@ -3800,10 +3797,10 @@
         <v>1</v>
       </c>
       <c r="J91" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K91" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
@@ -3835,15 +3832,15 @@
         <v>1</v>
       </c>
       <c r="J92" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K92" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B93" t="s">
         <v>11</v>
@@ -3870,15 +3867,15 @@
         <v>0</v>
       </c>
       <c r="J93" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K93" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B94" t="s">
         <v>11</v>
@@ -3905,15 +3902,15 @@
         <v>0</v>
       </c>
       <c r="J94" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="K94" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B95" t="s">
         <v>11</v>
@@ -3940,15 +3937,15 @@
         <v>0</v>
       </c>
       <c r="J95" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K95" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B96" t="s">
         <v>12</v>
@@ -3975,15 +3972,15 @@
         <v>0</v>
       </c>
       <c r="J96" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K96" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B97" t="s">
         <v>12</v>
@@ -4010,15 +4007,15 @@
         <v>0</v>
       </c>
       <c r="J97" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K97" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B98" t="s">
         <v>12</v>
@@ -4045,15 +4042,15 @@
         <v>0</v>
       </c>
       <c r="J98" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K98" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B99" t="s">
         <v>13</v>
@@ -4080,15 +4077,15 @@
         <v>0</v>
       </c>
       <c r="J99" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K99" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B100" t="s">
         <v>13</v>
@@ -4115,15 +4112,15 @@
         <v>0</v>
       </c>
       <c r="J100" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K100" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B101" t="s">
         <v>13</v>
@@ -4150,15 +4147,15 @@
         <v>0</v>
       </c>
       <c r="J101" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="K101" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B102" t="s">
         <v>13</v>
@@ -4185,15 +4182,15 @@
         <v>0</v>
       </c>
       <c r="J102" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K102" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B103" t="s">
         <v>13</v>
@@ -4220,15 +4217,15 @@
         <v>0</v>
       </c>
       <c r="J103" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K103" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B104" t="s">
         <v>13</v>
@@ -4249,21 +4246,21 @@
         <v>-3</v>
       </c>
       <c r="H104" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I104" t="b">
         <v>0</v>
       </c>
       <c r="J104" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K104" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B105" t="s">
         <v>17</v>
@@ -4284,21 +4281,21 @@
         <v>0</v>
       </c>
       <c r="H105" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I105" t="b">
         <v>0</v>
       </c>
       <c r="J105" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K105" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B106" t="s">
         <v>17</v>
@@ -4325,15 +4322,15 @@
         <v>0</v>
       </c>
       <c r="J106" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K106" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B107" t="s">
         <v>17</v>
@@ -4360,15 +4357,15 @@
         <v>0</v>
       </c>
       <c r="J107" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K107" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B108" t="s">
         <v>17</v>
@@ -4395,15 +4392,15 @@
         <v>0</v>
       </c>
       <c r="J108" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K108" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B109" t="s">
         <v>18</v>
@@ -4430,15 +4427,15 @@
         <v>0</v>
       </c>
       <c r="J109" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K109" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B110" t="s">
         <v>18</v>
@@ -4465,15 +4462,15 @@
         <v>0</v>
       </c>
       <c r="J110" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K110" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B111" t="s">
         <v>18</v>
@@ -4500,15 +4497,15 @@
         <v>0</v>
       </c>
       <c r="J111" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K111" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B112" t="s">
         <v>18</v>
@@ -4535,15 +4532,15 @@
         <v>0</v>
       </c>
       <c r="J112" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K112" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B113" t="s">
         <v>19</v>
@@ -4570,15 +4567,15 @@
         <v>0</v>
       </c>
       <c r="J113" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K113" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B114" t="s">
         <v>19</v>
@@ -4605,15 +4602,15 @@
         <v>0</v>
       </c>
       <c r="J114" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K114" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B115" t="s">
         <v>19</v>
@@ -4640,15 +4637,15 @@
         <v>0</v>
       </c>
       <c r="J115" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K115" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B116" t="s">
         <v>19</v>
@@ -4675,15 +4672,15 @@
         <v>0</v>
       </c>
       <c r="J116" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K116" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B117" t="s">
         <v>19</v>
@@ -4710,15 +4707,15 @@
         <v>0</v>
       </c>
       <c r="J117" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K117" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B118" t="s">
         <v>19</v>
@@ -4745,15 +4742,15 @@
         <v>0</v>
       </c>
       <c r="J118" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K118" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B119" t="s">
         <v>19</v>
@@ -4780,15 +4777,15 @@
         <v>0</v>
       </c>
       <c r="J119" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K119" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B120" t="s">
         <v>19</v>
@@ -4809,21 +4806,21 @@
         <v>0</v>
       </c>
       <c r="H120" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I120" t="b">
         <v>0</v>
       </c>
       <c r="J120" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K120" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B121" t="s">
         <v>20</v>
@@ -4844,21 +4841,21 @@
         <v>0</v>
       </c>
       <c r="H121" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I121" t="b">
         <v>0</v>
       </c>
       <c r="J121" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K121" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B122" t="s">
         <v>20</v>
@@ -4885,15 +4882,15 @@
         <v>0</v>
       </c>
       <c r="J122" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K122" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B123" t="s">
         <v>20</v>
@@ -4920,15 +4917,15 @@
         <v>0</v>
       </c>
       <c r="J123" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K123" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B124" t="s">
         <v>20</v>
@@ -4955,15 +4952,15 @@
         <v>0</v>
       </c>
       <c r="J124" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K124" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B125" t="s">
         <v>21</v>
@@ -4990,15 +4987,15 @@
         <v>0</v>
       </c>
       <c r="J125" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K125" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B126" t="s">
         <v>21</v>
@@ -5025,15 +5022,15 @@
         <v>0</v>
       </c>
       <c r="J126" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K126" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B127" t="s">
         <v>21</v>
@@ -5060,15 +5057,15 @@
         <v>0</v>
       </c>
       <c r="J127" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K127" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B128" t="s">
         <v>22</v>
@@ -5095,15 +5092,15 @@
         <v>1</v>
       </c>
       <c r="J128" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K128" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B129" t="s">
         <v>22</v>
@@ -5130,15 +5127,15 @@
         <v>1</v>
       </c>
       <c r="J129" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K129" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B130" t="s">
         <v>22</v>
@@ -5165,15 +5162,15 @@
         <v>1</v>
       </c>
       <c r="J130" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K130" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B131" t="s">
         <v>22</v>
@@ -5200,15 +5197,15 @@
         <v>1</v>
       </c>
       <c r="J131" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K131" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B132" t="s">
         <v>22</v>
@@ -5235,15 +5232,15 @@
         <v>1</v>
       </c>
       <c r="J132" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K132" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B133" t="s">
         <v>22</v>
@@ -5270,15 +5267,15 @@
         <v>1</v>
       </c>
       <c r="J133" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K133" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B134" t="s">
         <v>22</v>
@@ -5305,15 +5302,15 @@
         <v>1</v>
       </c>
       <c r="J134" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K134" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B135" t="s">
         <v>22</v>
@@ -5340,15 +5337,15 @@
         <v>1</v>
       </c>
       <c r="J135" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K135" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B136" t="s">
         <v>22</v>
@@ -5375,15 +5372,15 @@
         <v>1</v>
       </c>
       <c r="J136" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K136" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B137" t="s">
         <v>22</v>
@@ -5410,15 +5407,15 @@
         <v>1</v>
       </c>
       <c r="J137" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K137" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B138" t="s">
         <v>22</v>
@@ -5445,15 +5442,15 @@
         <v>1</v>
       </c>
       <c r="J138" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K138" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B139" t="s">
         <v>22</v>
@@ -5480,15 +5477,15 @@
         <v>1</v>
       </c>
       <c r="J139" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K139" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B140" t="s">
         <v>22</v>
@@ -5515,15 +5512,15 @@
         <v>1</v>
       </c>
       <c r="J140" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K140" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B141" t="s">
         <v>22</v>
@@ -5550,15 +5547,15 @@
         <v>1</v>
       </c>
       <c r="J141" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K141" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B142" t="s">
         <v>22</v>
@@ -5585,15 +5582,15 @@
         <v>1</v>
       </c>
       <c r="J142" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K142" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B143" t="s">
         <v>22</v>
@@ -5620,15 +5617,15 @@
         <v>1</v>
       </c>
       <c r="J143" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K143" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B144" t="s">
         <v>22</v>
@@ -5655,15 +5652,15 @@
         <v>1</v>
       </c>
       <c r="J144" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K144" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B145" t="s">
         <v>22</v>
@@ -5690,15 +5687,15 @@
         <v>1</v>
       </c>
       <c r="J145" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K145" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B146" t="s">
         <v>22</v>
@@ -5725,15 +5722,15 @@
         <v>1</v>
       </c>
       <c r="J146" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K146" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B147" t="s">
         <v>22</v>
@@ -5760,15 +5757,15 @@
         <v>1</v>
       </c>
       <c r="J147" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K147" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B148" t="s">
         <v>22</v>
@@ -5795,15 +5792,15 @@
         <v>1</v>
       </c>
       <c r="J148" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K148" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B149" t="s">
         <v>22</v>
@@ -5824,21 +5821,21 @@
         <v>0</v>
       </c>
       <c r="H149" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I149" t="b">
         <v>1</v>
       </c>
       <c r="J149" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K149" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B150" t="s">
         <v>23</v>
@@ -5859,21 +5856,21 @@
         <v>0</v>
       </c>
       <c r="H150" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I150" t="b">
         <v>0</v>
       </c>
       <c r="J150" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K150" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B151" t="s">
         <v>23</v>
@@ -5900,15 +5897,15 @@
         <v>0</v>
       </c>
       <c r="J151" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K151" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B152" t="s">
         <v>23</v>
@@ -5935,15 +5932,15 @@
         <v>0</v>
       </c>
       <c r="J152" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K152" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B153" t="s">
         <v>23</v>
@@ -5970,15 +5967,15 @@
         <v>0</v>
       </c>
       <c r="J153" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K153" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B154" t="s">
         <v>23</v>
@@ -6005,15 +6002,15 @@
         <v>0</v>
       </c>
       <c r="J154" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K154" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B155" t="s">
         <v>24</v>
@@ -6040,15 +6037,15 @@
         <v>0</v>
       </c>
       <c r="J155" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K155" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B156" t="s">
         <v>24</v>
@@ -6075,15 +6072,15 @@
         <v>0</v>
       </c>
       <c r="J156" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K156" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B157" t="s">
         <v>24</v>
@@ -6110,15 +6107,15 @@
         <v>0</v>
       </c>
       <c r="J157" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K157" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B158" t="s">
         <v>24</v>
@@ -6145,15 +6142,15 @@
         <v>0</v>
       </c>
       <c r="J158" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K158" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B159" t="s">
         <v>24</v>
@@ -6180,15 +6177,15 @@
         <v>0</v>
       </c>
       <c r="J159" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K159" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B160" t="s">
         <v>24</v>
@@ -6215,15 +6212,15 @@
         <v>0</v>
       </c>
       <c r="J160" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K160" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B161" t="s">
         <v>25</v>
@@ -6250,15 +6247,15 @@
         <v>0</v>
       </c>
       <c r="J161" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K161" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B162" t="s">
         <v>25</v>
@@ -6285,15 +6282,15 @@
         <v>0</v>
       </c>
       <c r="J162" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K162" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B163" t="s">
         <v>25</v>
@@ -6320,15 +6317,15 @@
         <v>0</v>
       </c>
       <c r="J163" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K163" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B164" t="s">
         <v>25</v>
@@ -6355,15 +6352,15 @@
         <v>0</v>
       </c>
       <c r="J164" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K164" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B165" t="s">
         <v>25</v>
@@ -6390,15 +6387,15 @@
         <v>0</v>
       </c>
       <c r="J165" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K165" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B166" t="s">
         <v>26</v>
@@ -6425,15 +6422,15 @@
         <v>0</v>
       </c>
       <c r="J166" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K166" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B167" t="s">
         <v>26</v>
@@ -6460,15 +6457,15 @@
         <v>0</v>
       </c>
       <c r="J167" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K167" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B168" t="s">
         <v>26</v>
@@ -6489,21 +6486,21 @@
         <v>0</v>
       </c>
       <c r="H168" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I168" t="b">
         <v>0</v>
       </c>
       <c r="J168" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K168" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B169" t="s">
         <v>27</v>
@@ -6524,21 +6521,21 @@
         <v>0</v>
       </c>
       <c r="H169" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I169" t="b">
         <v>0</v>
       </c>
       <c r="J169" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K169" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B170" t="s">
         <v>27</v>
@@ -6565,15 +6562,15 @@
         <v>0</v>
       </c>
       <c r="J170" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K170" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B171" t="s">
         <v>27</v>
@@ -6600,15 +6597,15 @@
         <v>0</v>
       </c>
       <c r="J171" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K171" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B172" t="s">
         <v>27</v>
@@ -6635,15 +6632,15 @@
         <v>0</v>
       </c>
       <c r="J172" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K172" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B173" t="s">
         <v>27</v>
@@ -6670,15 +6667,15 @@
         <v>0</v>
       </c>
       <c r="J173" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K173" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B174" t="s">
         <v>27</v>
@@ -6705,15 +6702,15 @@
         <v>0</v>
       </c>
       <c r="J174" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K174" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B175" t="s">
         <v>27</v>
@@ -6740,15 +6737,15 @@
         <v>0</v>
       </c>
       <c r="J175" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K175" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B176" t="s">
         <v>27</v>
@@ -6775,15 +6772,15 @@
         <v>0</v>
       </c>
       <c r="J176" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K176" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B177" t="s">
         <v>27</v>
@@ -6810,15 +6807,15 @@
         <v>0</v>
       </c>
       <c r="J177" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K177" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B178" t="s">
         <v>28</v>
@@ -6845,15 +6842,15 @@
         <v>0</v>
       </c>
       <c r="J178" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K178" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B179" t="s">
         <v>28</v>
@@ -6880,15 +6877,15 @@
         <v>0</v>
       </c>
       <c r="J179" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K179" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B180" t="s">
         <v>28</v>
@@ -6915,15 +6912,15 @@
         <v>0</v>
       </c>
       <c r="J180" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K180" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B181" t="s">
         <v>29</v>
@@ -6950,15 +6947,15 @@
         <v>0</v>
       </c>
       <c r="J181" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K181" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B182" t="s">
         <v>29</v>
@@ -6985,15 +6982,15 @@
         <v>0</v>
       </c>
       <c r="J182" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K182" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B183" t="s">
         <v>29</v>
@@ -7020,15 +7017,15 @@
         <v>0</v>
       </c>
       <c r="J183" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K183" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B184" t="s">
         <v>29</v>
@@ -7055,15 +7052,15 @@
         <v>0</v>
       </c>
       <c r="J184" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K184" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B185" t="s">
         <v>29</v>
@@ -7090,15 +7087,15 @@
         <v>0</v>
       </c>
       <c r="J185" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K185" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B186" t="s">
         <v>29</v>
@@ -7125,15 +7122,15 @@
         <v>0</v>
       </c>
       <c r="J186" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K186" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B187" t="s">
         <v>29</v>
@@ -7160,15 +7157,15 @@
         <v>0</v>
       </c>
       <c r="J187" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K187" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B188" t="s">
         <v>29</v>
@@ -7195,15 +7192,15 @@
         <v>0</v>
       </c>
       <c r="J188" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K188" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B189" t="s">
         <v>29</v>
@@ -7230,15 +7227,15 @@
         <v>0</v>
       </c>
       <c r="J189" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K189" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B190" t="s">
         <v>30</v>
@@ -7265,15 +7262,15 @@
         <v>0</v>
       </c>
       <c r="J190" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K190" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B191" t="s">
         <v>30</v>
@@ -7300,15 +7297,15 @@
         <v>0</v>
       </c>
       <c r="J191" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K191" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B192" t="s">
         <v>30</v>
@@ -7335,15 +7332,15 @@
         <v>0</v>
       </c>
       <c r="J192" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K192" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B193" t="s">
         <v>31</v>
@@ -7370,15 +7367,15 @@
         <v>0</v>
       </c>
       <c r="J193" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K193" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B194" t="s">
         <v>32</v>
@@ -7405,15 +7402,15 @@
         <v>0</v>
       </c>
       <c r="J194" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K194" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B195" t="s">
         <v>32</v>
@@ -7440,15 +7437,15 @@
         <v>0</v>
       </c>
       <c r="J195" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K195" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B196" t="s">
         <v>32</v>
@@ -7475,15 +7472,15 @@
         <v>0</v>
       </c>
       <c r="J196" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K196" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B197" t="s">
         <v>33</v>
@@ -7510,15 +7507,15 @@
         <v>0</v>
       </c>
       <c r="J197" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K197" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B198" t="s">
         <v>33</v>
@@ -7545,15 +7542,15 @@
         <v>0</v>
       </c>
       <c r="J198" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K198" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B199" t="s">
         <v>33</v>
@@ -7580,15 +7577,15 @@
         <v>0</v>
       </c>
       <c r="J199" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K199" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B200" t="s">
         <v>33</v>
@@ -7615,15 +7612,15 @@
         <v>0</v>
       </c>
       <c r="J200" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K200" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B201" t="s">
         <v>33</v>
@@ -7650,18 +7647,18 @@
         <v>0</v>
       </c>
       <c r="J201" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K201" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
+        <v>42</v>
+      </c>
+      <c r="B202" t="s">
         <v>43</v>
-      </c>
-      <c r="B202" t="s">
-        <v>44</v>
       </c>
       <c r="C202">
         <v>110</v>
@@ -7685,18 +7682,18 @@
         <v>0</v>
       </c>
       <c r="J202" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K202" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
+        <v>42</v>
+      </c>
+      <c r="B203" t="s">
         <v>43</v>
-      </c>
-      <c r="B203" t="s">
-        <v>44</v>
       </c>
       <c r="C203">
         <v>111</v>
@@ -7720,18 +7717,18 @@
         <v>0</v>
       </c>
       <c r="J203" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K203" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
+        <v>42</v>
+      </c>
+      <c r="B204" t="s">
         <v>43</v>
-      </c>
-      <c r="B204" t="s">
-        <v>44</v>
       </c>
       <c r="C204">
         <v>112</v>
@@ -7755,18 +7752,18 @@
         <v>0</v>
       </c>
       <c r="J204" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K204" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
+        <v>42</v>
+      </c>
+      <c r="B205" t="s">
         <v>43</v>
-      </c>
-      <c r="B205" t="s">
-        <v>44</v>
       </c>
       <c r="C205">
         <v>113</v>
@@ -7790,18 +7787,18 @@
         <v>0</v>
       </c>
       <c r="J205" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K205" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
+        <v>42</v>
+      </c>
+      <c r="B206" t="s">
         <v>43</v>
-      </c>
-      <c r="B206" t="s">
-        <v>44</v>
       </c>
       <c r="C206">
         <v>114</v>
@@ -7825,18 +7822,18 @@
         <v>0</v>
       </c>
       <c r="J206" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K206" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
+        <v>42</v>
+      </c>
+      <c r="B207" t="s">
         <v>43</v>
-      </c>
-      <c r="B207" t="s">
-        <v>44</v>
       </c>
       <c r="C207">
         <v>115</v>
@@ -7860,18 +7857,18 @@
         <v>0</v>
       </c>
       <c r="J207" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K207" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
+        <v>42</v>
+      </c>
+      <c r="B208" t="s">
         <v>43</v>
-      </c>
-      <c r="B208" t="s">
-        <v>44</v>
       </c>
       <c r="C208">
         <v>116</v>
@@ -7895,18 +7892,18 @@
         <v>0</v>
       </c>
       <c r="J208" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K208" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B209" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C209">
         <v>117</v>
@@ -7930,18 +7927,18 @@
         <v>0</v>
       </c>
       <c r="J209" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K209" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B210" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C210">
         <v>118</v>
@@ -7965,18 +7962,18 @@
         <v>0</v>
       </c>
       <c r="J210" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K210" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B211" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C211">
         <v>119</v>
@@ -8000,18 +7997,18 @@
         <v>0</v>
       </c>
       <c r="J211" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K211" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B212" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C212">
         <v>120</v>
@@ -8035,18 +8032,18 @@
         <v>0</v>
       </c>
       <c r="J212" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K212" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B213" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C213">
         <v>121</v>
@@ -8070,18 +8067,18 @@
         <v>0</v>
       </c>
       <c r="J213" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K213" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B214" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C214">
         <v>122</v>
@@ -8105,18 +8102,18 @@
         <v>1</v>
       </c>
       <c r="J214" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K214" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B215" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C215">
         <v>123</v>
@@ -8140,18 +8137,18 @@
         <v>1</v>
       </c>
       <c r="J215" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K215" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B216" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C216">
         <v>124</v>
@@ -8175,18 +8172,18 @@
         <v>1</v>
       </c>
       <c r="J216" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K216" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B217" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C217">
         <v>125</v>
@@ -8210,18 +8207,18 @@
         <v>1</v>
       </c>
       <c r="J217" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K217" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B218" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C218">
         <v>126</v>
@@ -8245,18 +8242,18 @@
         <v>1</v>
       </c>
       <c r="J218" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K218" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B219" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C219">
         <v>127</v>
@@ -8280,18 +8277,18 @@
         <v>1</v>
       </c>
       <c r="J219" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K219" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B220" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C220">
         <v>128</v>
@@ -8315,18 +8312,18 @@
         <v>1</v>
       </c>
       <c r="J220" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K220" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B221" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C221">
         <v>129</v>
@@ -8350,18 +8347,18 @@
         <v>1</v>
       </c>
       <c r="J221" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K221" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B222" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C222">
         <v>130</v>
@@ -8385,18 +8382,18 @@
         <v>1</v>
       </c>
       <c r="J222" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K222" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B223" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C223">
         <v>131</v>
@@ -8420,18 +8417,18 @@
         <v>1</v>
       </c>
       <c r="J223" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K223" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B224" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C224">
         <v>132</v>
@@ -8455,18 +8452,18 @@
         <v>1</v>
       </c>
       <c r="J224" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K224" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B225" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C225">
         <v>133</v>
@@ -8490,18 +8487,18 @@
         <v>1</v>
       </c>
       <c r="J225" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K225" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B226" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C226">
         <v>134</v>
@@ -8525,18 +8522,18 @@
         <v>1</v>
       </c>
       <c r="J226" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K226" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B227" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C227">
         <v>135</v>
@@ -8560,18 +8557,18 @@
         <v>1</v>
       </c>
       <c r="J227" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K227" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B228" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C228">
         <v>136</v>
@@ -8595,18 +8592,18 @@
         <v>1</v>
       </c>
       <c r="J228" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K228" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B229" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C229">
         <v>137</v>
@@ -8630,18 +8627,18 @@
         <v>1</v>
       </c>
       <c r="J229" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K229" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B230" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C230">
         <v>138</v>
@@ -8665,18 +8662,18 @@
         <v>1</v>
       </c>
       <c r="J230" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K230" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B231" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C231">
         <v>139</v>
@@ -8700,18 +8697,18 @@
         <v>1</v>
       </c>
       <c r="J231" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K231" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B232" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C232">
         <v>140</v>
@@ -8735,18 +8732,18 @@
         <v>1</v>
       </c>
       <c r="J232" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K232" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B233" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C233">
         <v>141</v>
@@ -8770,18 +8767,18 @@
         <v>1</v>
       </c>
       <c r="J233" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K233" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B234" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C234">
         <v>142</v>
@@ -8805,18 +8802,18 @@
         <v>1</v>
       </c>
       <c r="J234" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K234" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B235" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C235">
         <v>143</v>
@@ -8840,18 +8837,18 @@
         <v>1</v>
       </c>
       <c r="J235" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K235" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B236" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C236">
         <v>144</v>
@@ -8875,18 +8872,18 @@
         <v>0</v>
       </c>
       <c r="J236" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K236" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B237" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C237">
         <v>145</v>
@@ -8910,18 +8907,18 @@
         <v>0</v>
       </c>
       <c r="J237" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K237" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B238" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C238">
         <v>146</v>
@@ -8945,18 +8942,18 @@
         <v>0</v>
       </c>
       <c r="J238" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K238" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B239" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C239">
         <v>147</v>
@@ -8980,18 +8977,18 @@
         <v>0</v>
       </c>
       <c r="J239" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K239" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B240" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C240">
         <v>148</v>
@@ -9015,18 +9012,18 @@
         <v>0</v>
       </c>
       <c r="J240" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K240" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="241" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B241" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C241">
         <v>149</v>
@@ -9050,18 +9047,18 @@
         <v>0</v>
       </c>
       <c r="J241" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K241" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="242" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B242" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C242">
         <v>150</v>
@@ -9085,10 +9082,10 @@
         <v>0</v>
       </c>
       <c r="J242" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K242" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added hw unit test, updated switches and lights. New PLC File
</commit_message>
<xml_diff>
--- a/track_model/block_information.xlsx
+++ b/track_model/block_information.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadin\Desktop\PlanesOverTrains\track_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmkla\Documents\College\Senior\Trains\PlanesOverTrains_V2\track_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2229E9D3-9F26-4AFE-A71A-C64721B9F5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F58A01-DF98-4F40-B14A-E3B7663FC4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B483B09-FFFC-4D34-ABD1-C01B931B0F20}"/>
   </bookViews>
@@ -602,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA592A9B-DE73-4643-A9BC-018E16FBEA2A}">
   <dimension ref="A1:K242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
-      <selection activeCell="J101" sqref="J101"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="H155" sqref="H155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5996,7 +5996,7 @@
         <v>0</v>
       </c>
       <c r="H154" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I154" t="b">
         <v>0</v>
@@ -6031,7 +6031,7 @@
         <v>0</v>
       </c>
       <c r="H155" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I155" t="b">
         <v>0</v>
@@ -6486,7 +6486,7 @@
         <v>0</v>
       </c>
       <c r="H168" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I168" t="b">
         <v>0</v>
@@ -6521,7 +6521,7 @@
         <v>0</v>
       </c>
       <c r="H169" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I169" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
switch position finally works, updated missing info in block_information.xlsx, added new switchionary to block_info.py
</commit_message>
<xml_diff>
--- a/track_model/block_information.xlsx
+++ b/track_model/block_information.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmkla\Documents\College\Senior\Trains\PlanesOverTrains_V2\track_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadin\Desktop\PlanesOverTrains\track_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F58A01-DF98-4F40-B14A-E3B7663FC4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D869A1AC-C039-4D82-9054-652E02C97C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B483B09-FFFC-4D34-ABD1-C01B931B0F20}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{2B483B09-FFFC-4D34-ABD1-C01B931B0F20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -602,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA592A9B-DE73-4643-A9BC-018E16FBEA2A}">
   <dimension ref="A1:K242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="H155" sqref="H155"/>
+    <sheetView tabSelected="1" topLeftCell="B190" workbookViewId="0">
+      <selection activeCell="K206" sqref="K206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7822,10 +7822,10 @@
         <v>0</v>
       </c>
       <c r="J206" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="K206" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="207" spans="1:11" x14ac:dyDescent="0.25">
@@ -8102,10 +8102,10 @@
         <v>1</v>
       </c>
       <c r="J214" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="K214" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="215" spans="1:11" x14ac:dyDescent="0.25">
@@ -8417,10 +8417,10 @@
         <v>1</v>
       </c>
       <c r="J223" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="K223" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="224" spans="1:11" x14ac:dyDescent="0.25">
@@ -8732,10 +8732,10 @@
         <v>1</v>
       </c>
       <c r="J232" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="K232" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="233" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed Some Excel Sheet Stuff
</commit_message>
<xml_diff>
--- a/track_model/block_information.xlsx
+++ b/track_model/block_information.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadin\Desktop\PlanesOverTrains\track_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmkla\Documents\College\Senior\Trains\PlanesOverTrains_V2\track_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D869A1AC-C039-4D82-9054-652E02C97C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF237E2-75FB-41C1-B62E-9489101F41F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{2B483B09-FFFC-4D34-ABD1-C01B931B0F20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B483B09-FFFC-4D34-ABD1-C01B931B0F20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -602,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA592A9B-DE73-4643-A9BC-018E16FBEA2A}">
   <dimension ref="A1:K242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B190" workbookViewId="0">
-      <selection activeCell="K206" sqref="K206"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="H121" sqref="H121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4246,7 +4246,7 @@
         <v>-3</v>
       </c>
       <c r="H104" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I104" t="b">
         <v>0</v>
@@ -4281,7 +4281,7 @@
         <v>0</v>
       </c>
       <c r="H105" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I105" t="b">
         <v>0</v>
@@ -4806,7 +4806,7 @@
         <v>0</v>
       </c>
       <c r="H120" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I120" t="b">
         <v>0</v>
@@ -4841,7 +4841,7 @@
         <v>0</v>
       </c>
       <c r="H121" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I121" t="b">
         <v>0</v>
@@ -5821,7 +5821,7 @@
         <v>0</v>
       </c>
       <c r="H149" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I149" t="b">
         <v>1</v>
@@ -5856,7 +5856,7 @@
         <v>0</v>
       </c>
       <c r="H150" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I150" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
added direction to track model UI, added entry on red switches in block info
</commit_message>
<xml_diff>
--- a/track_model/block_information.xlsx
+++ b/track_model/block_information.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmkla\Documents\College\Senior\Trains\PlanesOverTrains_V2\track_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadin\Desktop\PlanesOverTrains\track_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF237E2-75FB-41C1-B62E-9489101F41F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F03EBBA-7536-4C1B-9427-811A57875FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B483B09-FFFC-4D34-ABD1-C01B931B0F20}"/>
+    <workbookView xWindow="3075" yWindow="4245" windowWidth="21600" windowHeight="11235" xr2:uid="{2B483B09-FFFC-4D34-ABD1-C01B931B0F20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -600,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA592A9B-DE73-4643-A9BC-018E16FBEA2A}">
-  <dimension ref="A1:K242"/>
+  <dimension ref="A1:K243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="H121" sqref="H121"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K243" sqref="A243:K243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9088,6 +9088,10 @@
         <v>65</v>
       </c>
     </row>
+    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E243" s="1"/>
+      <c r="G243" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>